<commit_message>
Atualizado por script em 23-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/denmark_1st-division_2023-2024.xlsx
+++ b/2023/denmark_1st-division_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V96"/>
+  <dimension ref="A1:V97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9289,6 +9289,98 @@
         </is>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>denmark</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>1st-division</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>45253.79166666666</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Fredericia</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>B.93</t>
+        </is>
+      </c>
+      <c r="I97" t="n">
+        <v>4</v>
+      </c>
+      <c r="J97" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>15/11/2023 19:42</t>
+        </is>
+      </c>
+      <c r="L97" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>23/11/2023 18:58</t>
+        </is>
+      </c>
+      <c r="N97" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>15/11/2023 19:42</t>
+        </is>
+      </c>
+      <c r="P97" t="n">
+        <v>4.76</v>
+      </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>23/11/2023 18:58</t>
+        </is>
+      </c>
+      <c r="R97" t="n">
+        <v>7.16</v>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>15/11/2023 19:42</t>
+        </is>
+      </c>
+      <c r="T97" t="n">
+        <v>5.41</v>
+      </c>
+      <c r="U97" t="inlineStr">
+        <is>
+          <t>23/11/2023 18:58</t>
+        </is>
+      </c>
+      <c r="V97" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/denmark/1st-division/fredericia-boldklubben-1893/pMeVjKZp/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>